<commit_message>
bit packing functions tested and complete
</commit_message>
<xml_diff>
--- a/Datasheets/Register Map.xlsx
+++ b/Datasheets/Register Map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Projects\CAN_J1939 Tech Track Project\j1939_tech_track_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Projects\CAN_J1939 Tech Track Project\j1939_tech_track_project\Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C084EC-D30B-4838-B376-E544FA4D9CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626B78A0-AF7A-42DF-AB9A-9F19B2465D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36297246-6964-43A8-9FA3-9E19564CB728}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -518,6 +518,24 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -530,12 +548,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -552,19 +564,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -952,46 +951,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8FC8FD-4393-424B-93FD-195EFD579748}">
   <dimension ref="B1:AJ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AB23" sqref="AB23"/>
+    <sheetView tabSelected="1" topLeftCell="O3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" customWidth="1"/>
-    <col min="21" max="21" width="5.7109375" customWidth="1"/>
-    <col min="22" max="23" width="5.85546875" customWidth="1"/>
-    <col min="24" max="24" width="5.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" customWidth="1"/>
+    <col min="21" max="21" width="5.6640625" customWidth="1"/>
+    <col min="22" max="23" width="5.88671875" customWidth="1"/>
+    <col min="24" max="24" width="5.6640625" customWidth="1"/>
     <col min="25" max="25" width="6" customWidth="1"/>
-    <col min="26" max="26" width="6.28515625" customWidth="1"/>
-    <col min="27" max="27" width="4.7109375" customWidth="1"/>
-    <col min="28" max="28" width="4.85546875" customWidth="1"/>
-    <col min="29" max="30" width="5.140625" customWidth="1"/>
+    <col min="26" max="26" width="6.33203125" customWidth="1"/>
+    <col min="27" max="27" width="4.6640625" customWidth="1"/>
+    <col min="28" max="28" width="4.88671875" customWidth="1"/>
+    <col min="29" max="30" width="5.109375" customWidth="1"/>
     <col min="31" max="31" width="5" customWidth="1"/>
-    <col min="32" max="32" width="5.42578125" customWidth="1"/>
+    <col min="32" max="32" width="5.44140625" customWidth="1"/>
     <col min="33" max="33" width="6" customWidth="1"/>
-    <col min="34" max="34" width="5.140625" customWidth="1"/>
-    <col min="35" max="35" width="6.42578125" customWidth="1"/>
-    <col min="36" max="36" width="5.85546875" customWidth="1"/>
+    <col min="34" max="34" width="5.109375" customWidth="1"/>
+    <col min="35" max="35" width="6.44140625" customWidth="1"/>
+    <col min="36" max="36" width="5.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1049,7 +1048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1072,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1095,21 +1094,21 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="21"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="25"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1138,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1167,7 +1166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1196,7 +1195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1225,21 +1224,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="24"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1268,7 +1267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1326,7 +1325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
@@ -1365,47 +1364,40 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
-      <c r="T19" s="16" t="s">
+      <c r="T19" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="U19" s="17"/>
-      <c r="V19" s="17"/>
-      <c r="W19" s="17"/>
-      <c r="X19" s="17"/>
-      <c r="Y19" s="17"/>
-      <c r="Z19" s="17"/>
-      <c r="AA19" s="17"/>
-      <c r="AB19" s="18"/>
-      <c r="AC19" s="17" t="s">
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="14"/>
+      <c r="X19" s="14"/>
+      <c r="Y19" s="14"/>
+      <c r="Z19" s="14"/>
+      <c r="AA19" s="14"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="AD19" s="17"/>
-      <c r="AE19" s="17"/>
-      <c r="AF19" s="17"/>
-      <c r="AG19" s="17"/>
-      <c r="AH19" s="17"/>
-      <c r="AI19" s="17"/>
-      <c r="AJ19" s="18"/>
-    </row>
-    <row r="20" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
+      <c r="AD19" s="14"/>
+      <c r="AE19" s="14"/>
+      <c r="AF19" s="14"/>
+      <c r="AG19" s="14"/>
+      <c r="AH19" s="14"/>
+      <c r="AI19" s="14"/>
+      <c r="AJ19" s="15"/>
+    </row>
+    <row r="20" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="B20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="25"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
       <c r="T20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1458,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1486,13 +1478,6 @@
       <c r="J21" s="10">
         <v>0</v>
       </c>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
       <c r="T21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1545,7 +1530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1573,13 +1558,12 @@
       <c r="J22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="M22" s="25"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
       <c r="T22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1626,7 +1610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1654,13 +1638,12 @@
       <c r="J23" s="10">
         <v>9</v>
       </c>
-      <c r="M23" s="25"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
       <c r="T23" s="2" t="s">
         <v>11</v>
       </c>
@@ -1707,7 +1690,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
@@ -1735,42 +1718,31 @@
       <c r="J24" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
-      <c r="U24" s="25"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="25"/>
-    </row>
-    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="T25" s="27" t="s">
+    </row>
+    <row r="25" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="T25" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="U25" s="28"/>
-      <c r="V25" s="28"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="28"/>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="28"/>
-      <c r="AA25" s="28"/>
-      <c r="AB25" s="29"/>
-      <c r="AC25" s="28" t="s">
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="17"/>
+      <c r="AA25" s="17"/>
+      <c r="AB25" s="18"/>
+      <c r="AC25" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="AD25" s="28"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
-      <c r="AG25" s="28"/>
-      <c r="AH25" s="28"/>
-      <c r="AI25" s="28"/>
-      <c r="AJ25" s="29"/>
-    </row>
-    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AD25" s="17"/>
+      <c r="AE25" s="17"/>
+      <c r="AF25" s="17"/>
+      <c r="AG25" s="17"/>
+      <c r="AH25" s="17"/>
+      <c r="AI25" s="17"/>
+      <c r="AJ25" s="18"/>
+    </row>
+    <row r="26" spans="2:36" x14ac:dyDescent="0.3">
       <c r="T26" s="1" t="s">
         <v>22</v>
       </c>
@@ -1823,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:36" x14ac:dyDescent="0.3">
       <c r="T27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1876,7 +1848,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:36" x14ac:dyDescent="0.3">
       <c r="T28" s="1" t="s">
         <v>23</v>
       </c>
@@ -1929,7 +1901,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="T29" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>